<commit_message>
Update to the experiments figures.
</commit_message>
<xml_diff>
--- a/extensions/fractionalUpdating-August2016/experiments/SimulatedDataExp-Normal.xlsx
+++ b/extensions/fractionalUpdating-August2016/experiments/SimulatedDataExp-Normal.xlsx
@@ -13,8 +13,9 @@
     <sheet name="Chart5" sheetId="7" r:id="rId4"/>
     <sheet name="Chart6" sheetId="8" r:id="rId5"/>
     <sheet name="Chart1" sheetId="9" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId8"/>
+    <sheet name="Chart7" sheetId="10" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>SVBFading-0.9</t>
   </si>
@@ -46,9 +47,6 @@
     <t>SVB-HPP</t>
   </si>
   <si>
-    <t>E[\RHO]</t>
-  </si>
-  <si>
     <t>Population-100-0.1</t>
   </si>
   <si>
@@ -62,6 +60,15 @@
   </si>
   <si>
     <t>SVBFading-0.99</t>
+  </si>
+  <si>
+    <t>SVB-HPP-Batch1000</t>
+  </si>
+  <si>
+    <t>E[\RHO]-Batch1000</t>
+  </si>
+  <si>
+    <t>E[\RHO]-Batch100</t>
   </si>
 </sst>
 </file>
@@ -110,8 +117,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -179,7 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -211,6 +220,7 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -242,6 +252,7 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6230,7 +6241,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>E[\RHO]</c:v>
+                  <c:v>E[\RHO]-Batch100</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9308,6 +9319,735 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$U$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>E[\RHO]-Batch100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$U$2:$U$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="103"/>
+                <c:pt idx="1">
+                  <c:v>0.932458447105444</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9336625245918</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.937466718143879</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.937921036477667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.938933660227807</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.939296594287549</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.938836859358978</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.940117608521869</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.93907841484728</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.938957598509437</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.940796746413844</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.94061984485455</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.940771690880668</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.94120016018377</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.940268074595841</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.94115050835561</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.941698381500656</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.941575684818818</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.940454327138601</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.94117140448075</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.941853065666146</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.940549656028602</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.942116217807236</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.942053003006029</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.942216270905057</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.942420518143381</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.942364124176555</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.941660161471345</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.942277485481259</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.942553786042928</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.942448216870134</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.942600240558759</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="0.00E+00">
+                  <c:v>0.000412578141624243</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.932439187221237</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.93437151706137</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.936083472719972</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.93821601655992</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.938695856841496</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.938416263849419</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.939810612285011</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.940114675573013</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.939849051260495</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.940303136475978</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.940392487468826</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.940676879928224</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.939390875441405</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.941326391923674</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.94095823376851</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.941418275458666</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.941024321684661</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.94177947497211</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.941500958013722</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.942040234627578</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.942058153167165</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.942002882319277</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.942232278888369</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.942209211386102</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.94229173436655</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.941064371933426</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.942405062884659</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.941675786082139</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.942484021627119</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.942528803779888</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.942491634390441</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.942605467258972</c:v>
+                </c:pt>
+                <c:pt idx="66" formatCode="0.00E+00">
+                  <c:v>0.000286942979859448</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.934328572381728</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.93642633766023</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.936906017811515</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.93224048251029</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.938140077691267</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.938991497293613</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.93863538489665</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.93982476898893</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.940123547726514</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.940458544407415</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.94040129883512</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.940729877617739</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.94069769720361</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.941028692213946</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.941517799604364</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.94152879837219</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.941661563101775</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.941349235871502</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.941285569870348</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.942012495807498</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.941745052774357</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.942104966708912</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.942108831763473</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.942293548106621</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.942370742269309</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.942314227923649</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.941970665537843</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.942171877315923</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.942382165554833</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.942515856232273</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.942477024943183</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.941681278947305</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.942657424735112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AS$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>E[\RHO]-Batch1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AS$2:$AS$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="103"/>
+                <c:pt idx="1">
+                  <c:v>0.942383153968453</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.943901821456816</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.945399815860031</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94555350056628</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.946440913242275</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.946097230080087</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.944033652574061</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.947385726734862</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.947553929497529</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.947560306306275</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.947968358692954</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.947363968495005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.948312425861331</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.947750420187036</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.948019506035087</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.948436124524412</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.948694651281312</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.948713832045783</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.948792480663738</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.948473653691033</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.948864659453841</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.948531324879464</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.948460483609528</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.949226422844427</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.949237163457681</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.948893665902646</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.949374202845023</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.94918397736179</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.949419293206908</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.94951276470085</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.949211218152798</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.949402011385897</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="0.00E+00">
+                  <c:v>3.1854784476279E-5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.941940312126625</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.940840925654866</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.945282347618972</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.94584667227246</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.945575379321234</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.94680853323274</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.947144657871731</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.947336106600498</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.947592764801523</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.947539610875602</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.947679104959624</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.947237223412816</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.948178390329472</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.948079783796878</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.947772932733651</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.948672584287215</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.948460577315108</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.948309265357923</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.948591494621253</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.948984183382798</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.948583306674736</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.948699270183597</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.949183540577971</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.948990651279629</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.949237668575353</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.949288400333029</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.949350129465985</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.948862237540628</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.949420394313863</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.94947842220266</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.949344729411272</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.949490333981806</c:v>
+                </c:pt>
+                <c:pt idx="66" formatCode="0.00E+00">
+                  <c:v>2.89982072729921E-5</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.942321273060341</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.943564034967418</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.945170479732895</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.944000710977177</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.944934380170657</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.946052016046434</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.946901691076001</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.947342585321502</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.947400052369355</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.947737972788731</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.947631620241163</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.947995213441644</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.948128659750009</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.947943024514399</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.948429659241782</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.948573169247401</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.948419791093376</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.948809655356053</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.948678193379854</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.948790090232986</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.948564771459413</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.949106308917142</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.948939105824551</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.9492176331821</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.949202024826103</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.949285939370512</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.94885506228075</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.949372260594614</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.949217570833353</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.949430660464283</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.949242390790303</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.949407763456003</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.949606589623186</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2101732696"/>
+        <c:axId val="-2138992216"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2101732696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2138992216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2138992216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2101732696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
@@ -9364,6 +10104,17 @@
 </file>
 
 <file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="137" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
@@ -9510,6 +10261,33 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9214453" cy="5626934"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -9858,10 +10636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL104"/>
+  <dimension ref="A1:AS104"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AS3" sqref="AS3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9870,7 +10648,7 @@
     <col min="6" max="6" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:45">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -9890,22 +10668,28 @@
         <v>5</v>
       </c>
       <c r="U1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH1" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC1" t="s">
+      <c r="AL1" t="s">
         <v>10</v>
       </c>
-      <c r="AH1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AL1" t="s">
+      <c r="AR1" t="s">
         <v>11</v>
       </c>
+      <c r="AS1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:45">
       <c r="A2">
         <v>-142.40558668468501</v>
       </c>
@@ -9969,8 +10753,17 @@
       <c r="AL2">
         <v>-1.13658562385671</v>
       </c>
+      <c r="AP2">
+        <v>-1437.8180522656201</v>
+      </c>
+      <c r="AQ2">
+        <v>-1</v>
+      </c>
+      <c r="AR2">
+        <v>-0.98992799786868602</v>
+      </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:45">
       <c r="A3">
         <v>-124.950950391804</v>
       </c>
@@ -10037,8 +10830,20 @@
       <c r="AL3">
         <v>-1.04917221369044</v>
       </c>
+      <c r="AP3">
+        <v>-1391.9826308751899</v>
+      </c>
+      <c r="AQ3">
+        <v>-1</v>
+      </c>
+      <c r="AR3">
+        <v>-0.99521103355335205</v>
+      </c>
+      <c r="AS3">
+        <v>0.94238315396845296</v>
+      </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:45">
       <c r="A4">
         <v>-135.64322773185501</v>
       </c>
@@ -10105,8 +10910,20 @@
       <c r="AL4">
         <v>-1.0334904721756899</v>
       </c>
+      <c r="AP4">
+        <v>-1365.47129783778</v>
+      </c>
+      <c r="AQ4">
+        <v>-1</v>
+      </c>
+      <c r="AR4">
+        <v>-0.99220590270672604</v>
+      </c>
+      <c r="AS4">
+        <v>0.943901821456816</v>
+      </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:45">
       <c r="A5">
         <v>-139.08996529753699</v>
       </c>
@@ -10173,8 +10990,20 @@
       <c r="AL5">
         <v>-1.0170569925669799</v>
       </c>
+      <c r="AP5">
+        <v>-1412.1397804617</v>
+      </c>
+      <c r="AQ5">
+        <v>-1</v>
+      </c>
+      <c r="AR5">
+        <v>-0.99027653305795704</v>
+      </c>
+      <c r="AS5">
+        <v>0.94539981586003097</v>
+      </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:45">
       <c r="A6">
         <v>-144.656914412368</v>
       </c>
@@ -10241,8 +11070,20 @@
       <c r="AL6">
         <v>-1.0026719548335901</v>
       </c>
+      <c r="AP6">
+        <v>-1430.0276716052799</v>
+      </c>
+      <c r="AQ6">
+        <v>-1</v>
+      </c>
+      <c r="AR6">
+        <v>-0.99939894034334398</v>
+      </c>
+      <c r="AS6">
+        <v>0.94555350056627996</v>
+      </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:45">
       <c r="A7">
         <v>-129.53714886915</v>
       </c>
@@ -10309,8 +11150,20 @@
       <c r="AL7">
         <v>-1.00073383147058</v>
       </c>
+      <c r="AP7">
+        <v>-1390.9162522905101</v>
+      </c>
+      <c r="AQ7">
+        <v>-1</v>
+      </c>
+      <c r="AR7">
+        <v>-1.0028319260959599</v>
+      </c>
+      <c r="AS7">
+        <v>0.94644091324227497</v>
+      </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:45">
       <c r="A8">
         <v>-147.51140281861001</v>
       </c>
@@ -10377,8 +11230,20 @@
       <c r="AL8">
         <v>-1.0058655587476</v>
       </c>
+      <c r="AP8">
+        <v>-1429.61753088053</v>
+      </c>
+      <c r="AQ8">
+        <v>-1</v>
+      </c>
+      <c r="AR8">
+        <v>-0.99335227740253795</v>
+      </c>
+      <c r="AS8">
+        <v>0.94609723008008695</v>
+      </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:45">
       <c r="A9">
         <v>-157.78518208680001</v>
       </c>
@@ -10445,8 +11310,20 @@
       <c r="AL9">
         <v>-1.02472677912211</v>
       </c>
+      <c r="AP9">
+        <v>-1429.2378517305001</v>
+      </c>
+      <c r="AQ9">
+        <v>-1</v>
+      </c>
+      <c r="AR9">
+        <v>-1.0049671415981201</v>
+      </c>
+      <c r="AS9">
+        <v>0.94403365257406102</v>
+      </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:45">
       <c r="A10">
         <v>-144.350269736494</v>
       </c>
@@ -10513,8 +11390,20 @@
       <c r="AL10">
         <v>-1.0201273013738901</v>
       </c>
+      <c r="AP10">
+        <v>-1421.39870537108</v>
+      </c>
+      <c r="AQ10">
+        <v>-1</v>
+      </c>
+      <c r="AR10">
+        <v>-1.0069094599222901</v>
+      </c>
+      <c r="AS10">
+        <v>0.94738572673486199</v>
+      </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:45">
       <c r="A11">
         <v>-139.360607660797</v>
       </c>
@@ -10581,8 +11470,20 @@
       <c r="AL11">
         <v>-1.0093271292935799</v>
       </c>
+      <c r="AP11">
+        <v>-1403.06002268882</v>
+      </c>
+      <c r="AQ11">
+        <v>-1</v>
+      </c>
+      <c r="AR11">
+        <v>-1.0067563711504901</v>
+      </c>
+      <c r="AS11">
+        <v>0.94755392949752903</v>
+      </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:45">
       <c r="A12">
         <v>-148.415814778852</v>
       </c>
@@ -10649,8 +11550,20 @@
       <c r="AL12">
         <v>-1.01065996005901</v>
       </c>
+      <c r="AP12">
+        <v>-1406.1491022888399</v>
+      </c>
+      <c r="AQ12">
+        <v>-1</v>
+      </c>
+      <c r="AR12">
+        <v>-1.00906954337405</v>
+      </c>
+      <c r="AS12">
+        <v>0.94756030630627497</v>
+      </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:45">
       <c r="A13">
         <v>-135.80339326497199</v>
       </c>
@@ -10717,8 +11630,20 @@
       <c r="AL13">
         <v>-1.01376560547324</v>
       </c>
+      <c r="AP13">
+        <v>-1425.6322454559499</v>
+      </c>
+      <c r="AQ13">
+        <v>-1</v>
+      </c>
+      <c r="AR13">
+        <v>-1.0062489054403201</v>
+      </c>
+      <c r="AS13">
+        <v>0.94796835869295404</v>
+      </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:45">
       <c r="A14">
         <v>-142.043797634697</v>
       </c>
@@ -10785,8 +11710,20 @@
       <c r="AL14">
         <v>-1.0261404402025001</v>
       </c>
+      <c r="AP14">
+        <v>-1412.11281797928</v>
+      </c>
+      <c r="AQ14">
+        <v>-1</v>
+      </c>
+      <c r="AR14">
+        <v>-1.00414398696075</v>
+      </c>
+      <c r="AS14">
+        <v>0.94736396849500504</v>
+      </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:45">
       <c r="A15">
         <v>-146.319593834561</v>
       </c>
@@ -10853,8 +11790,20 @@
       <c r="AL15">
         <v>-1.0193209604676099</v>
       </c>
+      <c r="AP15">
+        <v>-1377.49218754309</v>
+      </c>
+      <c r="AQ15">
+        <v>-1</v>
+      </c>
+      <c r="AR15">
+        <v>-1.0044123089405299</v>
+      </c>
+      <c r="AS15">
+        <v>0.94831242586133102</v>
+      </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:45">
       <c r="A16">
         <v>-144.727687290669</v>
       </c>
@@ -10921,8 +11870,20 @@
       <c r="AL16">
         <v>-1.0246681438441501</v>
       </c>
+      <c r="AP16">
+        <v>-1435.2842018696499</v>
+      </c>
+      <c r="AQ16">
+        <v>-1</v>
+      </c>
+      <c r="AR16">
+        <v>-1.00990805182814</v>
+      </c>
+      <c r="AS16">
+        <v>0.94775042018703604</v>
+      </c>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:45">
       <c r="A17">
         <v>-144.052186728707</v>
       </c>
@@ -10989,8 +11950,20 @@
       <c r="AL17">
         <v>-1.0128498553440799</v>
       </c>
+      <c r="AP17">
+        <v>-1421.1435251024</v>
+      </c>
+      <c r="AQ17">
+        <v>-1</v>
+      </c>
+      <c r="AR17">
+        <v>-1.00360551199054</v>
+      </c>
+      <c r="AS17">
+        <v>0.948019506035087</v>
+      </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:45">
       <c r="A18">
         <v>-130.63410909975099</v>
       </c>
@@ -11057,8 +12030,20 @@
       <c r="AL18">
         <v>-1.0243316977977499</v>
       </c>
+      <c r="AP18">
+        <v>-1388.6065954579699</v>
+      </c>
+      <c r="AQ18">
+        <v>-1</v>
+      </c>
+      <c r="AR18">
+        <v>-1.0074920194044701</v>
+      </c>
+      <c r="AS18">
+        <v>0.94843612452441195</v>
+      </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:45">
       <c r="A19">
         <v>-142.167086227456</v>
       </c>
@@ -11125,8 +12110,20 @@
       <c r="AL19">
         <v>-1.02365969383887</v>
       </c>
+      <c r="AP19">
+        <v>-1430.86221106218</v>
+      </c>
+      <c r="AQ19">
+        <v>-1</v>
+      </c>
+      <c r="AR19">
+        <v>-1.0068821310809699</v>
+      </c>
+      <c r="AS19">
+        <v>0.94869465128131203</v>
+      </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:45">
       <c r="A20">
         <v>-140.581130461859</v>
       </c>
@@ -11193,8 +12190,20 @@
       <c r="AL20">
         <v>-1.0184213609964201</v>
       </c>
+      <c r="AP20">
+        <v>-1429.42816059083</v>
+      </c>
+      <c r="AQ20">
+        <v>-1</v>
+      </c>
+      <c r="AR20">
+        <v>-1.00989420773248</v>
+      </c>
+      <c r="AS20">
+        <v>0.94871383204578297</v>
+      </c>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:45">
       <c r="A21">
         <v>-140.15537830582099</v>
       </c>
@@ -11261,8 +12270,20 @@
       <c r="AL21">
         <v>-1.01004899140689</v>
       </c>
+      <c r="AP21">
+        <v>-1408.4545406202601</v>
+      </c>
+      <c r="AQ21">
+        <v>-1</v>
+      </c>
+      <c r="AR21">
+        <v>-1.00678195530936</v>
+      </c>
+      <c r="AS21">
+        <v>0.948792480663738</v>
+      </c>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:45">
       <c r="A22">
         <v>-140.16207830703101</v>
       </c>
@@ -11329,8 +12350,20 @@
       <c r="AL22">
         <v>-0.99894632336514799</v>
       </c>
+      <c r="AP22">
+        <v>-1435.0547170699399</v>
+      </c>
+      <c r="AQ22">
+        <v>-1</v>
+      </c>
+      <c r="AR22">
+        <v>-1.00417114220901</v>
+      </c>
+      <c r="AS22">
+        <v>0.94847365369103298</v>
+      </c>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:45">
       <c r="A23">
         <v>-141.728880018144</v>
       </c>
@@ -11397,8 +12430,20 @@
       <c r="AL23">
         <v>-0.99542264405652203</v>
       </c>
+      <c r="AP23">
+        <v>-1393.688345001</v>
+      </c>
+      <c r="AQ23">
+        <v>-1</v>
+      </c>
+      <c r="AR23">
+        <v>-1.00060180066491</v>
+      </c>
+      <c r="AS23">
+        <v>0.94886465945384102</v>
+      </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:45">
       <c r="A24">
         <v>-147.25466201856199</v>
       </c>
@@ -11465,8 +12510,20 @@
       <c r="AL24">
         <v>-0.97839654650330699</v>
       </c>
+      <c r="AP24">
+        <v>-1433.36155024555</v>
+      </c>
+      <c r="AQ24">
+        <v>-1</v>
+      </c>
+      <c r="AR24">
+        <v>-0.99485596235055096</v>
+      </c>
+      <c r="AS24">
+        <v>0.94853132487946401</v>
+      </c>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:45">
       <c r="A25">
         <v>-142.964327393551</v>
       </c>
@@ -11533,8 +12590,20 @@
       <c r="AL25">
         <v>-0.97878509968001803</v>
       </c>
+      <c r="AP25">
+        <v>-1466.7357655542</v>
+      </c>
+      <c r="AQ25">
+        <v>-1</v>
+      </c>
+      <c r="AR25">
+        <v>-0.99540080515873297</v>
+      </c>
+      <c r="AS25">
+        <v>0.94846048360952795</v>
+      </c>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:45">
       <c r="A26">
         <v>-162.344688876389</v>
       </c>
@@ -11601,8 +12670,20 @@
       <c r="AL26">
         <v>-0.97911421731539905</v>
       </c>
+      <c r="AP26">
+        <v>-1429.7643076798099</v>
+      </c>
+      <c r="AQ26">
+        <v>-1</v>
+      </c>
+      <c r="AR26">
+        <v>-0.99404727067802201</v>
+      </c>
+      <c r="AS26">
+        <v>0.94922642284442704</v>
+      </c>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:45">
       <c r="A27">
         <v>-141.842701822793</v>
       </c>
@@ -11669,8 +12750,20 @@
       <c r="AL27">
         <v>-0.97364514601081498</v>
       </c>
+      <c r="AP27">
+        <v>-1450.2541332549799</v>
+      </c>
+      <c r="AQ27">
+        <v>-1</v>
+      </c>
+      <c r="AR27">
+        <v>-0.99216278937500502</v>
+      </c>
+      <c r="AS27">
+        <v>0.94923716345768105</v>
+      </c>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:45">
       <c r="A28">
         <v>-142.452264315695</v>
       </c>
@@ -11737,8 +12830,20 @@
       <c r="AL28">
         <v>-0.97352535341074398</v>
       </c>
+      <c r="AP28">
+        <v>-1429.7630300347701</v>
+      </c>
+      <c r="AQ28">
+        <v>-1</v>
+      </c>
+      <c r="AR28">
+        <v>-0.99459807337862505</v>
+      </c>
+      <c r="AS28">
+        <v>0.94889366590264601</v>
+      </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:45">
       <c r="A29">
         <v>-144.781046285119</v>
       </c>
@@ -11805,8 +12910,20 @@
       <c r="AL29">
         <v>-0.975348416061671</v>
       </c>
+      <c r="AP29">
+        <v>-1419.6652381998099</v>
+      </c>
+      <c r="AQ29">
+        <v>-1</v>
+      </c>
+      <c r="AR29">
+        <v>-0.99496188337872704</v>
+      </c>
+      <c r="AS29">
+        <v>0.94937420284502305</v>
+      </c>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:45">
       <c r="A30">
         <v>-137.870263511357</v>
       </c>
@@ -11873,8 +12990,20 @@
       <c r="AL30">
         <v>-0.98509609509958496</v>
       </c>
+      <c r="AP30">
+        <v>-1423.2871742262701</v>
+      </c>
+      <c r="AQ30">
+        <v>-1</v>
+      </c>
+      <c r="AR30">
+        <v>-0.99854786011943397</v>
+      </c>
+      <c r="AS30">
+        <v>0.94918397736179005</v>
+      </c>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:45">
       <c r="A31">
         <v>-135.24239836592099</v>
       </c>
@@ -11941,8 +13070,20 @@
       <c r="AL31">
         <v>-0.98907826924559195</v>
       </c>
+      <c r="AP31">
+        <v>-1436.9560617107099</v>
+      </c>
+      <c r="AQ31">
+        <v>-1</v>
+      </c>
+      <c r="AR31">
+        <v>-0.99836689216100805</v>
+      </c>
+      <c r="AS31">
+        <v>0.94941929320690799</v>
+      </c>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:45">
       <c r="A32">
         <v>-149.351769331827</v>
       </c>
@@ -12009,8 +13150,20 @@
       <c r="AL32">
         <v>-0.98994004005710001</v>
       </c>
+      <c r="AP32">
+        <v>-1417.62606837766</v>
+      </c>
+      <c r="AQ32">
+        <v>-1</v>
+      </c>
+      <c r="AR32">
+        <v>-0.99829277144510098</v>
+      </c>
+      <c r="AS32">
+        <v>0.94951276470085</v>
+      </c>
     </row>
-    <row r="33" spans="1:38">
+    <row r="33" spans="1:45">
       <c r="A33">
         <v>-141.264524922281</v>
       </c>
@@ -12077,8 +13230,20 @@
       <c r="AL33">
         <v>-0.99469287494380698</v>
       </c>
+      <c r="AP33">
+        <v>-1464.5739559999699</v>
+      </c>
+      <c r="AQ33">
+        <v>-1</v>
+      </c>
+      <c r="AR33">
+        <v>-1.00216497926173</v>
+      </c>
+      <c r="AS33">
+        <v>0.94921121815279796</v>
+      </c>
     </row>
-    <row r="34" spans="1:38">
+    <row r="34" spans="1:45">
       <c r="A34">
         <v>-157.75205459448901</v>
       </c>
@@ -12145,8 +13310,20 @@
       <c r="AL34">
         <v>-0.99719659033054897</v>
       </c>
+      <c r="AP34">
+        <v>-1482.2356535680699</v>
+      </c>
+      <c r="AQ34">
+        <v>-1</v>
+      </c>
+      <c r="AR34">
+        <v>-1.0049482326403001</v>
+      </c>
+      <c r="AS34">
+        <v>0.94940201138589697</v>
+      </c>
     </row>
-    <row r="35" spans="1:38">
+    <row r="35" spans="1:45">
       <c r="A35">
         <v>-309.35468410602698</v>
       </c>
@@ -12213,8 +13390,20 @@
       <c r="AL35">
         <v>-0.92692066710145804</v>
       </c>
+      <c r="AP35">
+        <v>-1435.7471682605401</v>
+      </c>
+      <c r="AQ35">
+        <v>1</v>
+      </c>
+      <c r="AR35">
+        <v>0.98703958478759202</v>
+      </c>
+      <c r="AS35" s="1">
+        <v>3.1854784476278903E-5</v>
+      </c>
     </row>
-    <row r="36" spans="1:38">
+    <row r="36" spans="1:45">
       <c r="A36">
         <v>-267.45543232412598</v>
       </c>
@@ -12281,8 +13470,20 @@
       <c r="AL36">
         <v>-0.86019963637073804</v>
       </c>
+      <c r="AP36">
+        <v>-1410.5795839145001</v>
+      </c>
+      <c r="AQ36">
+        <v>1</v>
+      </c>
+      <c r="AR36">
+        <v>0.96873941703493305</v>
+      </c>
+      <c r="AS36">
+        <v>0.94194031212662499</v>
+      </c>
     </row>
-    <row r="37" spans="1:38">
+    <row r="37" spans="1:45">
       <c r="A37">
         <v>-289.01068794025502</v>
       </c>
@@ -12349,8 +13550,20 @@
       <c r="AL37">
         <v>-0.802716764926932</v>
       </c>
+      <c r="AP37">
+        <v>-1409.2500883585401</v>
+      </c>
+      <c r="AQ37">
+        <v>1</v>
+      </c>
+      <c r="AR37">
+        <v>1.00119969684097</v>
+      </c>
+      <c r="AS37">
+        <v>0.94084092565486599</v>
+      </c>
     </row>
-    <row r="38" spans="1:38">
+    <row r="38" spans="1:45">
       <c r="A38">
         <v>-252.984394593709</v>
       </c>
@@ -12417,8 +13630,20 @@
       <c r="AL38">
         <v>-0.74511671211735697</v>
       </c>
+      <c r="AP38">
+        <v>-1412.3677624132099</v>
+      </c>
+      <c r="AQ38">
+        <v>1</v>
+      </c>
+      <c r="AR38">
+        <v>1.0007773654319501</v>
+      </c>
+      <c r="AS38">
+        <v>0.94528234761897201</v>
+      </c>
     </row>
-    <row r="39" spans="1:38">
+    <row r="39" spans="1:45">
       <c r="A39">
         <v>-241.088258597883</v>
       </c>
@@ -12485,8 +13710,20 @@
       <c r="AL39">
         <v>-0.69180492465911203</v>
       </c>
+      <c r="AP39">
+        <v>-1408.1536713343201</v>
+      </c>
+      <c r="AQ39">
+        <v>1</v>
+      </c>
+      <c r="AR39">
+        <v>0.99464571367608001</v>
+      </c>
+      <c r="AS39">
+        <v>0.94584667227246</v>
+      </c>
     </row>
-    <row r="40" spans="1:38">
+    <row r="40" spans="1:45">
       <c r="A40">
         <v>-252.60660557954699</v>
       </c>
@@ -12553,8 +13790,20 @@
       <c r="AL40">
         <v>-0.64313203421134602</v>
       </c>
+      <c r="AP40">
+        <v>-1465.39346833542</v>
+      </c>
+      <c r="AQ40">
+        <v>1</v>
+      </c>
+      <c r="AR40">
+        <v>0.99278119127844999</v>
+      </c>
+      <c r="AS40">
+        <v>0.94557537932123403</v>
+      </c>
     </row>
-    <row r="41" spans="1:38">
+    <row r="41" spans="1:45">
       <c r="A41">
         <v>-245.481990541779</v>
       </c>
@@ -12621,8 +13870,20 @@
       <c r="AL41">
         <v>-0.59193942664069998</v>
       </c>
+      <c r="AP41">
+        <v>-1421.39554497569</v>
+      </c>
+      <c r="AQ41">
+        <v>1</v>
+      </c>
+      <c r="AR41">
+        <v>0.99508871698426604</v>
+      </c>
+      <c r="AS41">
+        <v>0.94680853323273995</v>
+      </c>
     </row>
-    <row r="42" spans="1:38">
+    <row r="42" spans="1:45">
       <c r="A42">
         <v>-212.48827215191201</v>
       </c>
@@ -12689,8 +13950,20 @@
       <c r="AL42">
         <v>-0.54521308113640299</v>
       </c>
+      <c r="AP42">
+        <v>-1420.7317455075799</v>
+      </c>
+      <c r="AQ42">
+        <v>1</v>
+      </c>
+      <c r="AR42">
+        <v>0.99229424627391405</v>
+      </c>
+      <c r="AS42">
+        <v>0.94714465787173097</v>
+      </c>
     </row>
-    <row r="43" spans="1:38">
+    <row r="43" spans="1:45">
       <c r="A43">
         <v>-232.477336952239</v>
       </c>
@@ -12757,8 +14030,20 @@
       <c r="AL43">
         <v>-0.49989936010657299</v>
       </c>
+      <c r="AP43">
+        <v>-1452.7690309548</v>
+      </c>
+      <c r="AQ43">
+        <v>1</v>
+      </c>
+      <c r="AR43">
+        <v>0.98858835329700601</v>
+      </c>
+      <c r="AS43">
+        <v>0.94733610660049805</v>
+      </c>
     </row>
-    <row r="44" spans="1:38">
+    <row r="44" spans="1:45">
       <c r="A44">
         <v>-206.79082462194901</v>
       </c>
@@ -12825,8 +14110,20 @@
       <c r="AL44">
         <v>-0.455485549900015</v>
       </c>
+      <c r="AP44">
+        <v>-1414.1434701954299</v>
+      </c>
+      <c r="AQ44">
+        <v>1</v>
+      </c>
+      <c r="AR44">
+        <v>0.99030902483083305</v>
+      </c>
+      <c r="AS44">
+        <v>0.94759276480152299</v>
+      </c>
     </row>
-    <row r="45" spans="1:38">
+    <row r="45" spans="1:45">
       <c r="A45">
         <v>-224.85196273808899</v>
       </c>
@@ -12893,8 +14190,20 @@
       <c r="AL45">
         <v>-0.41653485451953198</v>
       </c>
+      <c r="AP45">
+        <v>-1414.9336613619901</v>
+      </c>
+      <c r="AQ45">
+        <v>1</v>
+      </c>
+      <c r="AR45">
+        <v>0.98950254519194603</v>
+      </c>
+      <c r="AS45">
+        <v>0.94753961087560201</v>
+      </c>
     </row>
-    <row r="46" spans="1:38">
+    <row r="46" spans="1:45">
       <c r="A46">
         <v>-206.59938343128701</v>
       </c>
@@ -12961,8 +14270,20 @@
       <c r="AL46">
         <v>-0.37726059260712103</v>
       </c>
+      <c r="AP46">
+        <v>-1433.1136699594199</v>
+      </c>
+      <c r="AQ46">
+        <v>1</v>
+      </c>
+      <c r="AR46">
+        <v>0.98755794277808295</v>
+      </c>
+      <c r="AS46">
+        <v>0.94767910495962404</v>
+      </c>
     </row>
-    <row r="47" spans="1:38">
+    <row r="47" spans="1:45">
       <c r="A47">
         <v>-229.21476256085199</v>
       </c>
@@ -13029,8 +14350,20 @@
       <c r="AL47">
         <v>-0.341585097055983</v>
       </c>
+      <c r="AP47">
+        <v>-1431.5491385565001</v>
+      </c>
+      <c r="AQ47">
+        <v>1</v>
+      </c>
+      <c r="AR47">
+        <v>0.99118827058435199</v>
+      </c>
+      <c r="AS47">
+        <v>0.94723722341281602</v>
+      </c>
     </row>
-    <row r="48" spans="1:38">
+    <row r="48" spans="1:45">
       <c r="A48">
         <v>-198.239195222056</v>
       </c>
@@ -13097,8 +14430,20 @@
       <c r="AL48">
         <v>-0.30017876266022597</v>
       </c>
+      <c r="AP48">
+        <v>-1412.6395386694101</v>
+      </c>
+      <c r="AQ48">
+        <v>1</v>
+      </c>
+      <c r="AR48">
+        <v>0.99326912987292204</v>
+      </c>
+      <c r="AS48">
+        <v>0.94817839032947204</v>
+      </c>
     </row>
-    <row r="49" spans="1:38">
+    <row r="49" spans="1:45">
       <c r="A49">
         <v>-193.657912276145</v>
       </c>
@@ -13165,8 +14510,20 @@
       <c r="AL49">
         <v>-0.26657103759519302</v>
       </c>
+      <c r="AP49">
+        <v>-1427.18534394267</v>
+      </c>
+      <c r="AQ49">
+        <v>1</v>
+      </c>
+      <c r="AR49">
+        <v>0.99462693127510804</v>
+      </c>
+      <c r="AS49">
+        <v>0.94807978379687796</v>
+      </c>
     </row>
-    <row r="50" spans="1:38">
+    <row r="50" spans="1:45">
       <c r="A50">
         <v>-196.57279213267799</v>
       </c>
@@ -13233,8 +14590,20 @@
       <c r="AL50">
         <v>-0.236852444567314</v>
       </c>
+      <c r="AP50">
+        <v>-1387.7391556836201</v>
+      </c>
+      <c r="AQ50">
+        <v>1</v>
+      </c>
+      <c r="AR50">
+        <v>1.0009093094742001</v>
+      </c>
+      <c r="AS50">
+        <v>0.94777293273365104</v>
+      </c>
     </row>
-    <row r="51" spans="1:38">
+    <row r="51" spans="1:45">
       <c r="A51">
         <v>-192.97563770014699</v>
       </c>
@@ -13301,8 +14670,20 @@
       <c r="AL51">
         <v>-0.20381321279709799</v>
       </c>
+      <c r="AP51">
+        <v>-1413.97229633951</v>
+      </c>
+      <c r="AQ51">
+        <v>1</v>
+      </c>
+      <c r="AR51">
+        <v>1.0015374481067201</v>
+      </c>
+      <c r="AS51">
+        <v>0.94867258428721501</v>
+      </c>
     </row>
-    <row r="52" spans="1:38">
+    <row r="52" spans="1:45">
       <c r="A52">
         <v>-183.869914322038</v>
       </c>
@@ -13369,8 +14750,20 @@
       <c r="AL52">
         <v>-0.172372938947326</v>
       </c>
+      <c r="AP52">
+        <v>-1421.79935989244</v>
+      </c>
+      <c r="AQ52">
+        <v>1</v>
+      </c>
+      <c r="AR52">
+        <v>0.99867072301932702</v>
+      </c>
+      <c r="AS52">
+        <v>0.94846057731510802</v>
+      </c>
     </row>
-    <row r="53" spans="1:38">
+    <row r="53" spans="1:45">
       <c r="A53">
         <v>-203.72945134212799</v>
       </c>
@@ -13437,8 +14830,20 @@
       <c r="AL53">
         <v>-0.14172884941445699</v>
       </c>
+      <c r="AP53">
+        <v>-1420.9121946400401</v>
+      </c>
+      <c r="AQ53">
+        <v>1</v>
+      </c>
+      <c r="AR53">
+        <v>1.0044832261133501</v>
+      </c>
+      <c r="AS53">
+        <v>0.94830926535792304</v>
+      </c>
     </row>
-    <row r="54" spans="1:38">
+    <row r="54" spans="1:45">
       <c r="A54">
         <v>-191.67010768263901</v>
       </c>
@@ -13505,8 +14910,20 @@
       <c r="AL54">
         <v>-0.114813241214253</v>
       </c>
+      <c r="AP54">
+        <v>-1417.5175190172099</v>
+      </c>
+      <c r="AQ54">
+        <v>1</v>
+      </c>
+      <c r="AR54">
+        <v>1.00003586430386</v>
+      </c>
+      <c r="AS54">
+        <v>0.94859149462125303</v>
+      </c>
     </row>
-    <row r="55" spans="1:38">
+    <row r="55" spans="1:45">
       <c r="A55">
         <v>-184.26752116983801</v>
       </c>
@@ -13573,8 +14990,20 @@
       <c r="AL55">
         <v>-8.7633417806986594E-2</v>
       </c>
+      <c r="AP55">
+        <v>-1432.65006415384</v>
+      </c>
+      <c r="AQ55">
+        <v>1</v>
+      </c>
+      <c r="AR55">
+        <v>1.0014557933586199</v>
+      </c>
+      <c r="AS55">
+        <v>0.948984183382798</v>
+      </c>
     </row>
-    <row r="56" spans="1:38">
+    <row r="56" spans="1:45">
       <c r="A56">
         <v>-180.87214373684</v>
       </c>
@@ -13641,8 +15070,20 @@
       <c r="AL56">
         <v>-6.3481801816210104E-2</v>
       </c>
+      <c r="AP56">
+        <v>-1415.1377935667001</v>
+      </c>
+      <c r="AQ56">
+        <v>1</v>
+      </c>
+      <c r="AR56">
+        <v>0.99630803817802305</v>
+      </c>
+      <c r="AS56">
+        <v>0.948583306674736</v>
+      </c>
     </row>
-    <row r="57" spans="1:38">
+    <row r="57" spans="1:45">
       <c r="A57">
         <v>-185.94792147670699</v>
       </c>
@@ -13709,8 +15150,20 @@
       <c r="AL57">
         <v>-3.8006920336355103E-2</v>
       </c>
+      <c r="AP57">
+        <v>-1409.9404194501701</v>
+      </c>
+      <c r="AQ57">
+        <v>1</v>
+      </c>
+      <c r="AR57">
+        <v>0.99851969557592501</v>
+      </c>
+      <c r="AS57">
+        <v>0.94869927018359701</v>
+      </c>
     </row>
-    <row r="58" spans="1:38">
+    <row r="58" spans="1:45">
       <c r="A58">
         <v>-182.212824003073</v>
       </c>
@@ -13777,8 +15230,20 @@
       <c r="AL58">
         <v>-1.4133663375759799E-2</v>
       </c>
+      <c r="AP58">
+        <v>-1451.5929233849099</v>
+      </c>
+      <c r="AQ58">
+        <v>1</v>
+      </c>
+      <c r="AR58">
+        <v>0.99732902977554405</v>
+      </c>
+      <c r="AS58">
+        <v>0.94918354057797105</v>
+      </c>
     </row>
-    <row r="59" spans="1:38">
+    <row r="59" spans="1:45">
       <c r="A59">
         <v>-175.72161791314201</v>
       </c>
@@ -13845,8 +15310,20 @@
       <c r="AL59">
         <v>7.4985493713425203E-3</v>
       </c>
+      <c r="AP59">
+        <v>-1388.69940407987</v>
+      </c>
+      <c r="AQ59">
+        <v>1</v>
+      </c>
+      <c r="AR59">
+        <v>0.99404259399411399</v>
+      </c>
+      <c r="AS59">
+        <v>0.94899065127962901</v>
+      </c>
     </row>
-    <row r="60" spans="1:38">
+    <row r="60" spans="1:45">
       <c r="A60">
         <v>-176.888971939545</v>
       </c>
@@ -13913,8 +15390,20 @@
       <c r="AL60">
         <v>2.9915031930706801E-2</v>
       </c>
+      <c r="AP60">
+        <v>-1375.36207104708</v>
+      </c>
+      <c r="AQ60">
+        <v>1</v>
+      </c>
+      <c r="AR60">
+        <v>0.995645004616169</v>
+      </c>
+      <c r="AS60">
+        <v>0.94923766857535297</v>
+      </c>
     </row>
-    <row r="61" spans="1:38">
+    <row r="61" spans="1:45">
       <c r="A61">
         <v>-177.85462088672</v>
       </c>
@@ -13981,8 +15470,20 @@
       <c r="AL61">
         <v>4.4644057277182597E-2</v>
       </c>
+      <c r="AP61">
+        <v>-1404.7001242377801</v>
+      </c>
+      <c r="AQ61">
+        <v>1</v>
+      </c>
+      <c r="AR61">
+        <v>0.99383624083903799</v>
+      </c>
+      <c r="AS61">
+        <v>0.94928840033302897</v>
+      </c>
     </row>
-    <row r="62" spans="1:38">
+    <row r="62" spans="1:45">
       <c r="A62">
         <v>-185.72387173292799</v>
       </c>
@@ -14049,8 +15550,20 @@
       <c r="AL62">
         <v>6.4028078576465794E-2</v>
       </c>
+      <c r="AP62">
+        <v>-1401.33280532499</v>
+      </c>
+      <c r="AQ62">
+        <v>1</v>
+      </c>
+      <c r="AR62">
+        <v>0.99341734461545195</v>
+      </c>
+      <c r="AS62">
+        <v>0.94935012946598496</v>
+      </c>
     </row>
-    <row r="63" spans="1:38">
+    <row r="63" spans="1:45">
       <c r="A63">
         <v>-177.98202915074199</v>
       </c>
@@ -14117,8 +15630,20 @@
       <c r="AL63">
         <v>8.4952563933231501E-2</v>
       </c>
+      <c r="AP63">
+        <v>-1380.49349380733</v>
+      </c>
+      <c r="AQ63">
+        <v>1</v>
+      </c>
+      <c r="AR63">
+        <v>0.99126679168521104</v>
+      </c>
+      <c r="AS63">
+        <v>0.94886223754062804</v>
+      </c>
     </row>
-    <row r="64" spans="1:38">
+    <row r="64" spans="1:45">
       <c r="A64">
         <v>-169.849943765528</v>
       </c>
@@ -14185,8 +15710,20 @@
       <c r="AL64">
         <v>0.102324572683578</v>
       </c>
+      <c r="AP64">
+        <v>-1432.8546818786001</v>
+      </c>
+      <c r="AQ64">
+        <v>1</v>
+      </c>
+      <c r="AR64">
+        <v>0.99290183505900598</v>
+      </c>
+      <c r="AS64">
+        <v>0.94942039431386305</v>
+      </c>
     </row>
-    <row r="65" spans="1:38">
+    <row r="65" spans="1:45">
       <c r="A65">
         <v>-179.92801173574799</v>
       </c>
@@ -14253,8 +15790,20 @@
       <c r="AL65">
         <v>0.118951756702714</v>
       </c>
+      <c r="AP65">
+        <v>-1415.8828679897599</v>
+      </c>
+      <c r="AQ65">
+        <v>1</v>
+      </c>
+      <c r="AR65">
+        <v>0.99383234523713604</v>
+      </c>
+      <c r="AS65">
+        <v>0.94947842220265999</v>
+      </c>
     </row>
-    <row r="66" spans="1:38">
+    <row r="66" spans="1:45">
       <c r="A66">
         <v>-183.298031360072</v>
       </c>
@@ -14321,8 +15870,20 @@
       <c r="AL66">
         <v>0.135163150669562</v>
       </c>
+      <c r="AP66">
+        <v>-1420.7018319689901</v>
+      </c>
+      <c r="AQ66">
+        <v>1</v>
+      </c>
+      <c r="AR66">
+        <v>0.99393834202857101</v>
+      </c>
+      <c r="AS66">
+        <v>0.94934472941127201</v>
+      </c>
     </row>
-    <row r="67" spans="1:38">
+    <row r="67" spans="1:45">
       <c r="A67">
         <v>-176.697100274848</v>
       </c>
@@ -14389,8 +15950,20 @@
       <c r="AL67">
         <v>0.15186030782998</v>
       </c>
+      <c r="AP67">
+        <v>-1384.92263663619</v>
+      </c>
+      <c r="AQ67">
+        <v>1</v>
+      </c>
+      <c r="AR67">
+        <v>0.99454408714084697</v>
+      </c>
+      <c r="AS67">
+        <v>0.94949033398180605</v>
+      </c>
     </row>
-    <row r="68" spans="1:38">
+    <row r="68" spans="1:45">
       <c r="A68">
         <v>-170.56992306722299</v>
       </c>
@@ -14457,8 +16030,20 @@
       <c r="AL68">
         <v>0.127664936283201</v>
       </c>
+      <c r="AP68">
+        <v>-1436.5420057797701</v>
+      </c>
+      <c r="AQ68">
+        <v>-1</v>
+      </c>
+      <c r="AR68">
+        <v>-1.0177272848340799</v>
+      </c>
+      <c r="AS68" s="1">
+        <v>2.8998207272992101E-5</v>
+      </c>
     </row>
-    <row r="69" spans="1:38">
+    <row r="69" spans="1:45">
       <c r="A69">
         <v>-170.05524226909401</v>
       </c>
@@ -14525,8 +16110,20 @@
       <c r="AL69">
         <v>0.105360579446812</v>
       </c>
+      <c r="AP69">
+        <v>-1394.6009276365501</v>
+      </c>
+      <c r="AQ69">
+        <v>-1</v>
+      </c>
+      <c r="AR69">
+        <v>-1.0003195399092799</v>
+      </c>
+      <c r="AS69">
+        <v>0.94232127306034097</v>
+      </c>
     </row>
-    <row r="70" spans="1:38">
+    <row r="70" spans="1:45">
       <c r="A70">
         <v>-184.71455615590801</v>
       </c>
@@ -14593,8 +16190,20 @@
       <c r="AL70">
         <v>8.3318753692782202E-2</v>
       </c>
+      <c r="AP70">
+        <v>-1401.8107124876501</v>
+      </c>
+      <c r="AQ70">
+        <v>-1</v>
+      </c>
+      <c r="AR70">
+        <v>-0.99711187392773604</v>
+      </c>
+      <c r="AS70">
+        <v>0.94356403496741803</v>
+      </c>
     </row>
-    <row r="71" spans="1:38">
+    <row r="71" spans="1:45">
       <c r="A71">
         <v>-171.85846880619499</v>
       </c>
@@ -14661,8 +16270,20 @@
       <c r="AL71">
         <v>6.3244699465576398E-2</v>
       </c>
+      <c r="AP71">
+        <v>-1413.9292678735501</v>
+      </c>
+      <c r="AQ71">
+        <v>-1</v>
+      </c>
+      <c r="AR71">
+        <v>-0.993785745214253</v>
+      </c>
+      <c r="AS71">
+        <v>0.94517047973289503</v>
+      </c>
     </row>
-    <row r="72" spans="1:38">
+    <row r="72" spans="1:45">
       <c r="A72">
         <v>-172.91899519229801</v>
       </c>
@@ -14729,8 +16350,20 @@
       <c r="AL72">
         <v>3.8731376056302599E-2</v>
       </c>
+      <c r="AP72">
+        <v>-1442.46236804671</v>
+      </c>
+      <c r="AQ72">
+        <v>-1</v>
+      </c>
+      <c r="AR72">
+        <v>-1.01105126194203</v>
+      </c>
+      <c r="AS72">
+        <v>0.94400071097717697</v>
+      </c>
     </row>
-    <row r="73" spans="1:38">
+    <row r="73" spans="1:45">
       <c r="A73">
         <v>-175.01826871670701</v>
       </c>
@@ -14797,8 +16430,20 @@
       <c r="AL73">
         <v>2.02941970576485E-2</v>
       </c>
+      <c r="AP73">
+        <v>-1435.1124651141299</v>
+      </c>
+      <c r="AQ73">
+        <v>-1</v>
+      </c>
+      <c r="AR73">
+        <v>-1.0042720179326401</v>
+      </c>
+      <c r="AS73">
+        <v>0.94493438017065701</v>
+      </c>
     </row>
-    <row r="74" spans="1:38">
+    <row r="74" spans="1:45">
       <c r="A74">
         <v>-176.11108438606999</v>
       </c>
@@ -14865,8 +16510,20 @@
       <c r="AL74">
         <v>-1.2464539133110999E-3</v>
       </c>
+      <c r="AP74">
+        <v>-1428.07895647326</v>
+      </c>
+      <c r="AQ74">
+        <v>-1</v>
+      </c>
+      <c r="AR74">
+        <v>-0.99939401313782095</v>
+      </c>
+      <c r="AS74">
+        <v>0.94605201604643396</v>
+      </c>
     </row>
-    <row r="75" spans="1:38">
+    <row r="75" spans="1:45">
       <c r="A75">
         <v>-171.74314643998599</v>
       </c>
@@ -14933,8 +16590,20 @@
       <c r="AL75">
         <v>-1.9011202679617801E-2</v>
       </c>
+      <c r="AP75">
+        <v>-1417.6201946712099</v>
+      </c>
+      <c r="AQ75">
+        <v>-1</v>
+      </c>
+      <c r="AR75">
+        <v>-1.0005850584187701</v>
+      </c>
+      <c r="AS75">
+        <v>0.94690169107600097</v>
+      </c>
     </row>
-    <row r="76" spans="1:38">
+    <row r="76" spans="1:45">
       <c r="A76">
         <v>-159.55110418255401</v>
       </c>
@@ -15001,8 +16670,20 @@
       <c r="AL76">
         <v>-3.8434291349353902E-2</v>
       </c>
+      <c r="AP76">
+        <v>-1361.6866416083201</v>
+      </c>
+      <c r="AQ76">
+        <v>-1</v>
+      </c>
+      <c r="AR76">
+        <v>-0.99930277660338196</v>
+      </c>
+      <c r="AS76">
+        <v>0.94734258532150195</v>
+      </c>
     </row>
-    <row r="77" spans="1:38">
+    <row r="77" spans="1:45">
       <c r="A77">
         <v>-170.009649230186</v>
       </c>
@@ -15069,8 +16750,20 @@
       <c r="AL77">
         <v>-5.8807668705352499E-2</v>
       </c>
+      <c r="AP77">
+        <v>-1442.6247759885</v>
+      </c>
+      <c r="AQ77">
+        <v>-1</v>
+      </c>
+      <c r="AR77">
+        <v>-1.0018686164514901</v>
+      </c>
+      <c r="AS77">
+        <v>0.94740005236935498</v>
+      </c>
     </row>
-    <row r="78" spans="1:38">
+    <row r="78" spans="1:45">
       <c r="A78">
         <v>-169.93149056901899</v>
       </c>
@@ -15137,8 +16830,20 @@
       <c r="AL78">
         <v>-7.4969645937526405E-2</v>
       </c>
+      <c r="AP78">
+        <v>-1418.24733937272</v>
+      </c>
+      <c r="AQ78">
+        <v>-1</v>
+      </c>
+      <c r="AR78">
+        <v>-1.0029161802983799</v>
+      </c>
+      <c r="AS78">
+        <v>0.94773797278873095</v>
+      </c>
     </row>
-    <row r="79" spans="1:38">
+    <row r="79" spans="1:45">
       <c r="A79">
         <v>-171.71443550884899</v>
       </c>
@@ -15205,8 +16910,20 @@
       <c r="AL79">
         <v>-8.9919589660120605E-2</v>
       </c>
+      <c r="AP79">
+        <v>-1395.48927598829</v>
+      </c>
+      <c r="AQ79">
+        <v>-1</v>
+      </c>
+      <c r="AR79">
+        <v>-0.99685116160132703</v>
+      </c>
+      <c r="AS79">
+        <v>0.94763162024116299</v>
+      </c>
     </row>
-    <row r="80" spans="1:38">
+    <row r="80" spans="1:45">
       <c r="A80">
         <v>-165.79107273612601</v>
       </c>
@@ -15273,8 +16990,20 @@
       <c r="AL80">
         <v>-0.104290839843001</v>
       </c>
+      <c r="AP80">
+        <v>-1447.10928098162</v>
+      </c>
+      <c r="AQ80">
+        <v>-1</v>
+      </c>
+      <c r="AR80">
+        <v>-1.00094794925657</v>
+      </c>
+      <c r="AS80">
+        <v>0.94799521344164395</v>
+      </c>
     </row>
-    <row r="81" spans="1:38">
+    <row r="81" spans="1:45">
       <c r="A81">
         <v>-166.665331543061</v>
       </c>
@@ -15341,8 +17070,20 @@
       <c r="AL81">
         <v>-0.11902103710381801</v>
       </c>
+      <c r="AP81">
+        <v>-1422.61131369141</v>
+      </c>
+      <c r="AQ81">
+        <v>-1</v>
+      </c>
+      <c r="AR81">
+        <v>-0.998476116558913</v>
+      </c>
+      <c r="AS81">
+        <v>0.94812865975000904</v>
+      </c>
     </row>
-    <row r="82" spans="1:38">
+    <row r="82" spans="1:45">
       <c r="A82">
         <v>-177.27698710412699</v>
       </c>
@@ -15409,8 +17150,20 @@
       <c r="AL82">
         <v>-0.13660547869307299</v>
       </c>
+      <c r="AP82">
+        <v>-1417.3353712281</v>
+      </c>
+      <c r="AQ82">
+        <v>-1</v>
+      </c>
+      <c r="AR82">
+        <v>-1.00434250550469</v>
+      </c>
+      <c r="AS82">
+        <v>0.94794302451439905</v>
+      </c>
     </row>
-    <row r="83" spans="1:38">
+    <row r="83" spans="1:45">
       <c r="A83">
         <v>-168.699014205249</v>
       </c>
@@ -15477,8 +17230,20 @@
       <c r="AL83">
         <v>-0.15190642450536801</v>
       </c>
+      <c r="AP83">
+        <v>-1444.48020938024</v>
+      </c>
+      <c r="AQ83">
+        <v>-1</v>
+      </c>
+      <c r="AR83">
+        <v>-1.00723663788607</v>
+      </c>
+      <c r="AS83">
+        <v>0.94842965924178202</v>
+      </c>
     </row>
-    <row r="84" spans="1:38">
+    <row r="84" spans="1:45">
       <c r="A84">
         <v>-163.46826253551001</v>
       </c>
@@ -15545,8 +17310,20 @@
       <c r="AL84">
         <v>-0.16719208000574901</v>
       </c>
+      <c r="AP84">
+        <v>-1440.62379183644</v>
+      </c>
+      <c r="AQ84">
+        <v>-1</v>
+      </c>
+      <c r="AR84">
+        <v>-1.0069386753707199</v>
+      </c>
+      <c r="AS84">
+        <v>0.94857316924740098</v>
+      </c>
     </row>
-    <row r="85" spans="1:38">
+    <row r="85" spans="1:45">
       <c r="A85">
         <v>-168.751350616884</v>
       </c>
@@ -15613,8 +17390,20 @@
       <c r="AL85">
         <v>-0.18315403758804799</v>
       </c>
+      <c r="AP85">
+        <v>-1451.79941103701</v>
+      </c>
+      <c r="AQ85">
+        <v>-1</v>
+      </c>
+      <c r="AR85">
+        <v>-1.0067078207128799</v>
+      </c>
+      <c r="AS85">
+        <v>0.94841979109337604</v>
+      </c>
     </row>
-    <row r="86" spans="1:38">
+    <row r="86" spans="1:45">
       <c r="A86">
         <v>-170.294977426374</v>
       </c>
@@ -15681,8 +17470,20 @@
       <c r="AL86">
         <v>-0.19720553714362099</v>
       </c>
+      <c r="AP86">
+        <v>-1412.6137680624099</v>
+      </c>
+      <c r="AQ86">
+        <v>-1</v>
+      </c>
+      <c r="AR86">
+        <v>-1.0050180619570499</v>
+      </c>
+      <c r="AS86">
+        <v>0.94880965535605299</v>
+      </c>
     </row>
-    <row r="87" spans="1:38">
+    <row r="87" spans="1:45">
       <c r="A87">
         <v>-171.609392258886</v>
       </c>
@@ -15749,8 +17550,20 @@
       <c r="AL87">
         <v>-0.20759105668745001</v>
       </c>
+      <c r="AP87">
+        <v>-1415.80808563194</v>
+      </c>
+      <c r="AQ87">
+        <v>-1</v>
+      </c>
+      <c r="AR87">
+        <v>-1.0009759623074701</v>
+      </c>
+      <c r="AS87">
+        <v>0.94867819337985404</v>
+      </c>
     </row>
-    <row r="88" spans="1:38">
+    <row r="88" spans="1:45">
       <c r="A88">
         <v>-158.086441116402</v>
       </c>
@@ -15817,8 +17630,20 @@
       <c r="AL88">
         <v>-0.22171914303333301</v>
       </c>
+      <c r="AP88">
+        <v>-1474.57540685617</v>
+      </c>
+      <c r="AQ88">
+        <v>-1</v>
+      </c>
+      <c r="AR88">
+        <v>-1.00360625670042</v>
+      </c>
+      <c r="AS88">
+        <v>0.94879009023298599</v>
+      </c>
     </row>
-    <row r="89" spans="1:38">
+    <row r="89" spans="1:45">
       <c r="A89">
         <v>-165.52427751606601</v>
       </c>
@@ -15885,8 +17710,20 @@
       <c r="AL89">
         <v>-0.23576995556625099</v>
       </c>
+      <c r="AP89">
+        <v>-1413.12198585693</v>
+      </c>
+      <c r="AQ89">
+        <v>-1</v>
+      </c>
+      <c r="AR89">
+        <v>-1.0009231246249499</v>
+      </c>
+      <c r="AS89">
+        <v>0.94856477145941298</v>
+      </c>
     </row>
-    <row r="90" spans="1:38">
+    <row r="90" spans="1:45">
       <c r="A90">
         <v>-155.957835993727</v>
       </c>
@@ -15953,8 +17790,20 @@
       <c r="AL90">
         <v>-0.24748560654688301</v>
       </c>
+      <c r="AP90">
+        <v>-1447.5787954003799</v>
+      </c>
+      <c r="AQ90">
+        <v>-1</v>
+      </c>
+      <c r="AR90">
+        <v>-1.00220771857167</v>
+      </c>
+      <c r="AS90">
+        <v>0.94910630891714198</v>
+      </c>
     </row>
-    <row r="91" spans="1:38">
+    <row r="91" spans="1:45">
       <c r="A91">
         <v>-173.77662410414999</v>
       </c>
@@ -16021,8 +17870,20 @@
       <c r="AL91">
         <v>-0.26151674102549</v>
       </c>
+      <c r="AP91">
+        <v>-1420.6308455165599</v>
+      </c>
+      <c r="AQ91">
+        <v>-1</v>
+      </c>
+      <c r="AR91">
+        <v>-1.00564376026599</v>
+      </c>
+      <c r="AS91">
+        <v>0.94893910582455099</v>
+      </c>
     </row>
-    <row r="92" spans="1:38">
+    <row r="92" spans="1:45">
       <c r="A92">
         <v>-166.081775661324</v>
       </c>
@@ -16089,8 +17950,20 @@
       <c r="AL92">
         <v>-0.27360649727270298</v>
       </c>
+      <c r="AP92">
+        <v>-1402.5663122788501</v>
+      </c>
+      <c r="AQ92">
+        <v>-1</v>
+      </c>
+      <c r="AR92">
+        <v>-1.00501115077797</v>
+      </c>
+      <c r="AS92">
+        <v>0.94921763318209995</v>
+      </c>
     </row>
-    <row r="93" spans="1:38">
+    <row r="93" spans="1:45">
       <c r="A93">
         <v>-163.21301074990399</v>
       </c>
@@ -16157,8 +18030,20 @@
       <c r="AL93">
         <v>-0.28501597298356701</v>
       </c>
+      <c r="AP93">
+        <v>-1382.01277034952</v>
+      </c>
+      <c r="AQ93">
+        <v>-1</v>
+      </c>
+      <c r="AR93">
+        <v>-1.0032975709296099</v>
+      </c>
+      <c r="AS93">
+        <v>0.94920202482610305</v>
+      </c>
     </row>
-    <row r="94" spans="1:38">
+    <row r="94" spans="1:45">
       <c r="A94">
         <v>-163.151377191378</v>
       </c>
@@ -16225,8 +18110,20 @@
       <c r="AL94">
         <v>-0.29786931765431301</v>
       </c>
+      <c r="AP94">
+        <v>-1391.19883273235</v>
+      </c>
+      <c r="AQ94">
+        <v>-1</v>
+      </c>
+      <c r="AR94">
+        <v>-1.00525133051686</v>
+      </c>
+      <c r="AS94">
+        <v>0.94928593937051198</v>
+      </c>
     </row>
-    <row r="95" spans="1:38">
+    <row r="95" spans="1:45">
       <c r="A95">
         <v>-168.38207631504801</v>
       </c>
@@ -16293,8 +18190,20 @@
       <c r="AL95">
         <v>-0.30903952577420202</v>
       </c>
+      <c r="AP95">
+        <v>-1416.6736256134</v>
+      </c>
+      <c r="AQ95">
+        <v>-1</v>
+      </c>
+      <c r="AR95">
+        <v>-1.0075793236505399</v>
+      </c>
+      <c r="AS95">
+        <v>0.94885506228075001</v>
+      </c>
     </row>
-    <row r="96" spans="1:38">
+    <row r="96" spans="1:45">
       <c r="A96">
         <v>-168.94158240317799</v>
       </c>
@@ -16361,8 +18270,20 @@
       <c r="AL96">
         <v>-0.32092590471148302</v>
       </c>
+      <c r="AP96">
+        <v>-1448.82534570024</v>
+      </c>
+      <c r="AQ96">
+        <v>-1</v>
+      </c>
+      <c r="AR96">
+        <v>-1.0091843536805201</v>
+      </c>
+      <c r="AS96">
+        <v>0.94937226059461399</v>
+      </c>
     </row>
-    <row r="97" spans="1:38">
+    <row r="97" spans="1:45">
       <c r="A97">
         <v>-170.01860867008</v>
       </c>
@@ -16429,8 +18350,20 @@
       <c r="AL97">
         <v>-0.33196215408323898</v>
       </c>
+      <c r="AP97">
+        <v>-1446.8834623283201</v>
+      </c>
+      <c r="AQ97">
+        <v>-1</v>
+      </c>
+      <c r="AR97">
+        <v>-1.01031759217951</v>
+      </c>
+      <c r="AS97">
+        <v>0.94921757083335301</v>
+      </c>
     </row>
-    <row r="98" spans="1:38">
+    <row r="98" spans="1:45">
       <c r="A98">
         <v>-172.87290967916101</v>
       </c>
@@ -16497,8 +18430,20 @@
       <c r="AL98">
         <v>-0.34158968533159201</v>
       </c>
+      <c r="AP98">
+        <v>-1447.8554528427601</v>
+      </c>
+      <c r="AQ98">
+        <v>-1</v>
+      </c>
+      <c r="AR98">
+        <v>-1.0085786637895999</v>
+      </c>
+      <c r="AS98">
+        <v>0.94943066046428304</v>
+      </c>
     </row>
-    <row r="99" spans="1:38">
+    <row r="99" spans="1:45">
       <c r="A99">
         <v>-160.27482247896299</v>
       </c>
@@ -16565,8 +18510,20 @@
       <c r="AL99">
         <v>-0.35243304780253498</v>
       </c>
+      <c r="AP99">
+        <v>-1419.62895665426</v>
+      </c>
+      <c r="AQ99">
+        <v>-1</v>
+      </c>
+      <c r="AR99">
+        <v>-1.0079092864502299</v>
+      </c>
+      <c r="AS99">
+        <v>0.94924239079030304</v>
+      </c>
     </row>
-    <row r="100" spans="1:38">
+    <row r="100" spans="1:45">
       <c r="A100">
         <v>-162.01761229900001</v>
       </c>
@@ -16633,8 +18590,20 @@
       <c r="AL100">
         <v>-0.36350601575228703</v>
       </c>
+      <c r="AP100">
+        <v>-1416.5490890517599</v>
+      </c>
+      <c r="AQ100">
+        <v>-1</v>
+      </c>
+      <c r="AR100">
+        <v>-1.0088052006255599</v>
+      </c>
+      <c r="AS100">
+        <v>0.94940776345600297</v>
+      </c>
     </row>
-    <row r="101" spans="1:38">
+    <row r="101" spans="1:45">
       <c r="A101">
         <v>-163.40194799176399</v>
       </c>
@@ -16701,15 +18670,27 @@
       <c r="AL101">
         <v>-0.37242111980174297</v>
       </c>
+      <c r="AP101">
+        <v>-1419.87566662823</v>
+      </c>
+      <c r="AQ101">
+        <v>-1</v>
+      </c>
+      <c r="AR101">
+        <v>-1.00914244416821</v>
+      </c>
+      <c r="AS101">
+        <v>0.949606589623186</v>
+      </c>
     </row>
-    <row r="102" spans="1:38">
+    <row r="102" spans="1:45">
       <c r="AA102">
         <v>-6535.6691955387296</v>
       </c>
     </row>
-    <row r="104" spans="1:38">
+    <row r="104" spans="1:45">
       <c r="AA104" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>